<commit_message>
attempting to store player stats using classes because: dot notation
</commit_message>
<xml_diff>
--- a/assets/excel/ping_pong_scoresheet_v2.xlsx
+++ b/assets/excel/ping_pong_scoresheet_v2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="15">
   <si>
     <t>Fritz</t>
   </si>
@@ -191,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -206,6 +206,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1524,102 +1527,110 @@
         <v>5</v>
       </c>
     </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="4">
+        <v>43412</v>
+      </c>
+      <c r="B73" s="1">
+        <v>16</v>
+      </c>
+      <c r="C73" s="1">
+        <v>14</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="74" spans="1:4">
-      <c r="C74" s="2" t="s">
+      <c r="A74" s="4">
+        <v>43412</v>
+      </c>
+      <c r="B74" s="5">
+        <v>15</v>
+      </c>
+      <c r="C74" s="5">
+        <v>11</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="4">
+        <v>43412</v>
+      </c>
+      <c r="B75" s="1">
+        <v>15</v>
+      </c>
+      <c r="C75" s="1">
+        <v>3</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="4">
+        <v>43412</v>
+      </c>
+      <c r="B76" s="5">
+        <v>9</v>
+      </c>
+      <c r="C76" s="5">
+        <v>15</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="4">
+        <v>43412</v>
+      </c>
+      <c r="B77" s="1">
+        <v>7</v>
+      </c>
+      <c r="C77" s="1">
+        <v>15</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="4">
+        <v>43412</v>
+      </c>
+      <c r="B78" s="5">
+        <v>15</v>
+      </c>
+      <c r="C78" s="5">
+        <v>12</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="C80" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="2" t="s">
+    <row r="81" spans="1:4">
+      <c r="A81" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="1">
-        <v>15</v>
-      </c>
-      <c r="D75" s="1">
+      <c r="B81" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C76" s="1">
+      <c r="D81" s="1">
         <v>18</v>
-      </c>
-      <c r="D76" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C77" s="1">
-        <v>33</v>
-      </c>
-      <c r="D77" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="1">
-        <v>41.67</v>
-      </c>
-      <c r="D78" s="1">
-        <v>48.57</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C79" s="1">
-        <v>51.43</v>
-      </c>
-      <c r="D79" s="1">
-        <v>58.33</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C80" s="1">
-        <v>46.48</v>
-      </c>
-      <c r="D80" s="1">
-        <v>53.52</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="1">
-        <v>12.47</v>
-      </c>
-      <c r="D81" s="1">
-        <v>14.03</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1628,10 +1639,10 @@
         <v>4</v>
       </c>
       <c r="C82" s="1">
-        <v>13.69</v>
+        <v>20</v>
       </c>
       <c r="D82" s="1">
-        <v>13.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1640,44 +1651,120 @@
         <v>12</v>
       </c>
       <c r="C83" s="1">
-        <v>13.07</v>
+        <v>37</v>
       </c>
       <c r="D83" s="1">
-        <v>13.76</v>
+        <v>40</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C84" s="1">
-        <v>0</v>
+        <v>43.59</v>
       </c>
       <c r="D84" s="1">
-        <v>0</v>
+        <v>47.37</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2"/>
       <c r="B85" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="1">
+        <v>52.63</v>
+      </c>
+      <c r="D85" s="1">
+        <v>56.41</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" s="1">
+        <v>48.05</v>
+      </c>
+      <c r="D86" s="1">
+        <v>51.95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="1">
+        <v>12.49</v>
+      </c>
+      <c r="D87" s="1">
+        <v>13.92</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1">
+        <v>13.63</v>
+      </c>
+      <c r="D88" s="1">
+        <v>13.28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" s="1">
+        <v>13.05</v>
+      </c>
+      <c r="D89" s="1">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="1">
+        <v>1</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C85" s="1">
-        <v>0</v>
-      </c>
-      <c r="D85" s="1">
-        <v>0</v>
+      <c r="C91" s="1">
+        <v>4</v>
+      </c>
+      <c r="D91" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A78:A80"/>
     <mergeCell ref="A81:A83"/>
-    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A87:A89"/>
+    <mergeCell ref="A90:A91"/>
   </mergeCells>
   <conditionalFormatting sqref="B10">
     <cfRule type="cellIs" dxfId="0" priority="17" operator="greaterThan">
@@ -2024,6 +2111,36 @@
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B73">
+    <cfRule type="cellIs" dxfId="0" priority="143" operator="greaterThan">
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B74">
+    <cfRule type="cellIs" dxfId="0" priority="145" operator="greaterThan">
+      <formula>11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75">
+    <cfRule type="cellIs" dxfId="0" priority="147" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B76">
+    <cfRule type="cellIs" dxfId="0" priority="149" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B77">
+    <cfRule type="cellIs" dxfId="0" priority="151" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B78">
+    <cfRule type="cellIs" dxfId="0" priority="153" operator="greaterThan">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B8">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="greaterThan">
       <formula>10</formula>
@@ -2379,6 +2496,36 @@
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C73">
+    <cfRule type="cellIs" dxfId="0" priority="144" operator="greaterThan">
+      <formula>16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74">
+    <cfRule type="cellIs" dxfId="0" priority="146" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C75">
+    <cfRule type="cellIs" dxfId="0" priority="148" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C76">
+    <cfRule type="cellIs" dxfId="0" priority="150" operator="greaterThan">
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C77">
+    <cfRule type="cellIs" dxfId="0" priority="152" operator="greaterThan">
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C78">
+    <cfRule type="cellIs" dxfId="0" priority="154" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C8">
     <cfRule type="cellIs" dxfId="0" priority="14" operator="greaterThan">
       <formula>15</formula>

</xml_diff>

<commit_message>
building out classes; moving closer to dot notation
</commit_message>
<xml_diff>
--- a/assets/excel/ping_pong_scoresheet_v2.xlsx
+++ b/assets/excel/ping_pong_scoresheet_v2.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ktuten/Desktop/ping_pong/assets/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14417CC-5C19-5E43-A65E-C5F14EC2B508}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="15">
   <si>
     <t>Fritz</t>
   </si>
@@ -64,11 +70,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -209,11 +215,933 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="154">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -222,6 +1150,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -268,7 +1204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -300,9 +1236,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -334,6 +1288,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,17 +1481,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="1"/>
+    <col min="1" max="5" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -533,7 +1507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>43384</v>
       </c>
@@ -547,7 +1521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>43384</v>
       </c>
@@ -561,7 +1535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43384</v>
       </c>
@@ -575,7 +1549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>43384</v>
       </c>
@@ -589,7 +1563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>43384</v>
       </c>
@@ -603,7 +1577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>43384</v>
       </c>
@@ -617,7 +1591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>43384</v>
       </c>
@@ -631,7 +1605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>43384</v>
       </c>
@@ -645,7 +1619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>43384</v>
       </c>
@@ -659,7 +1633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>43384</v>
       </c>
@@ -673,7 +1647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>43384</v>
       </c>
@@ -687,7 +1661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>43384</v>
       </c>
@@ -701,7 +1675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>43384</v>
       </c>
@@ -715,7 +1689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>43384</v>
       </c>
@@ -729,7 +1703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>43384</v>
       </c>
@@ -743,7 +1717,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>43384</v>
       </c>
@@ -757,7 +1731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>43396</v>
       </c>
@@ -771,7 +1745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>43396</v>
       </c>
@@ -785,7 +1759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>43397</v>
       </c>
@@ -799,7 +1773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>43397</v>
       </c>
@@ -813,7 +1787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>43397</v>
       </c>
@@ -827,7 +1801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>43397</v>
       </c>
@@ -841,7 +1815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>43399</v>
       </c>
@@ -855,7 +1829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>43399</v>
       </c>
@@ -869,7 +1843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>43399</v>
       </c>
@@ -883,7 +1857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>43399</v>
       </c>
@@ -897,7 +1871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>43399</v>
       </c>
@@ -911,7 +1885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>43399</v>
       </c>
@@ -925,7 +1899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>43402</v>
       </c>
@@ -939,7 +1913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>43402</v>
       </c>
@@ -953,7 +1927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>43402</v>
       </c>
@@ -967,7 +1941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>43402</v>
       </c>
@@ -981,7 +1955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>43402</v>
       </c>
@@ -995,7 +1969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>43402</v>
       </c>
@@ -1009,7 +1983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>43402</v>
       </c>
@@ -1023,7 +1997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>43402</v>
       </c>
@@ -1037,7 +2011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>43402</v>
       </c>
@@ -1051,7 +2025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>43402</v>
       </c>
@@ -1065,7 +2039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>43402</v>
       </c>
@@ -1079,7 +2053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>43402</v>
       </c>
@@ -1093,7 +2067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>43402</v>
       </c>
@@ -1107,7 +2081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>43402</v>
       </c>
@@ -1121,7 +2095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43402</v>
       </c>
@@ -1135,7 +2109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>43402</v>
       </c>
@@ -1149,7 +2123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>43402</v>
       </c>
@@ -1163,7 +2137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>43402</v>
       </c>
@@ -1177,7 +2151,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>43402</v>
       </c>
@@ -1191,7 +2165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>43405</v>
       </c>
@@ -1205,7 +2179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>43405</v>
       </c>
@@ -1219,7 +2193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>43405</v>
       </c>
@@ -1233,7 +2207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>43409</v>
       </c>
@@ -1247,7 +2221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>43409</v>
       </c>
@@ -1261,7 +2235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>43409</v>
       </c>
@@ -1275,7 +2249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>43409</v>
       </c>
@@ -1289,7 +2263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>43409</v>
       </c>
@@ -1303,7 +2277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>43410</v>
       </c>
@@ -1317,7 +2291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>43410</v>
       </c>
@@ -1331,7 +2305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>43410</v>
       </c>
@@ -1345,7 +2319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>43410</v>
       </c>
@@ -1359,7 +2333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>43410</v>
       </c>
@@ -1373,7 +2347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>43410</v>
       </c>
@@ -1387,7 +2361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>43410</v>
       </c>
@@ -1401,7 +2375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>43410</v>
       </c>
@@ -1415,7 +2389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>43410</v>
       </c>
@@ -1429,7 +2403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>43411</v>
       </c>
@@ -1443,7 +2417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>43411</v>
       </c>
@@ -1457,7 +2431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>43411</v>
       </c>
@@ -1471,7 +2445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>43411</v>
       </c>
@@ -1485,7 +2459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>43411</v>
       </c>
@@ -1499,7 +2473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>43411</v>
       </c>
@@ -1513,7 +2487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>43411</v>
       </c>
@@ -1527,7 +2501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>43412</v>
       </c>
@@ -1541,7 +2515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>43412</v>
       </c>
@@ -1555,7 +2529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>43412</v>
       </c>
@@ -1569,7 +2543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>43412</v>
       </c>
@@ -1583,7 +2557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>43412</v>
       </c>
@@ -1597,7 +2571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>43412</v>
       </c>
@@ -1611,923 +2585,979 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="C80" s="2" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="10">
+        <v>43413</v>
+      </c>
+      <c r="B79" s="1">
+        <v>15</v>
+      </c>
+      <c r="C79" s="1">
+        <v>12</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="10">
+        <v>43413</v>
+      </c>
+      <c r="B80" s="1">
+        <v>16</v>
+      </c>
+      <c r="C80" s="1">
+        <v>18</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="10">
+        <v>43413</v>
+      </c>
+      <c r="B81" s="1">
+        <v>18</v>
+      </c>
+      <c r="C81" s="1">
+        <v>16</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="10">
+        <v>43413</v>
+      </c>
+      <c r="B82" s="1">
+        <v>16</v>
+      </c>
+      <c r="C82" s="1">
+        <v>14</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C84" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="8" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="1">
+      <c r="B85" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="1">
         <v>17</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D85" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C82" s="1">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="9"/>
+      <c r="B86" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" s="1">
         <v>20</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D86" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="9"/>
+      <c r="B87" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C87" s="1">
         <v>37</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D87" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="2" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="1">
+      <c r="B88" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="1">
         <v>43.59</v>
       </c>
-      <c r="D84" s="1">
+      <c r="D88" s="1">
         <v>47.37</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C85" s="1">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="9"/>
+      <c r="B89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" s="1">
         <v>52.63</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D89" s="1">
         <v>56.41</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="9"/>
+      <c r="B90" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C90" s="1">
         <v>48.05</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D90" s="1">
         <v>51.95</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="2" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="1">
+      <c r="B91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="1">
         <v>12.49</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D91" s="1">
         <v>13.92</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C88" s="1">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="9"/>
+      <c r="B92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" s="1">
         <v>13.63</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D92" s="1">
         <v>13.28</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="9"/>
+      <c r="B93" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C93" s="1">
         <v>13.05</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D93" s="1">
         <v>13.6</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="2" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C94" s="1">
         <v>1</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D94" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="2"/>
-      <c r="B91" s="2" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="9"/>
+      <c r="B95" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C91" s="1">
-        <v>4</v>
-      </c>
-      <c r="D91" s="1">
+      <c r="C95" s="1">
+        <v>4</v>
+      </c>
+      <c r="D95" s="1">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="A87:A89"/>
-    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="A94:A95"/>
   </mergeCells>
   <conditionalFormatting sqref="B10">
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="153" priority="17" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="cellIs" dxfId="0" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="152" priority="19" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="0" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="151" priority="21" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="0" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="150" priority="23" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="0" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="149" priority="25" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="cellIs" dxfId="0" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="27" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="cellIs" dxfId="0" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="29" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="cellIs" dxfId="0" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="146" priority="31" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="cellIs" dxfId="0" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="33" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="0" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="144" priority="35" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="143" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="0" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="37" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="0" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="141" priority="39" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="cellIs" dxfId="0" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="41" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="cellIs" dxfId="0" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="43" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="0" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="138" priority="45" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="cellIs" dxfId="0" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="137" priority="47" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="cellIs" dxfId="0" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="136" priority="49" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="0" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="51" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="0" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="53" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="0" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="55" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="3" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="0" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="57" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="cellIs" dxfId="0" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="59" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="0" priority="61" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="61" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="cellIs" dxfId="0" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="63" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="cellIs" dxfId="0" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="127" priority="65" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="cellIs" dxfId="0" priority="67" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="67" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="0" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="69" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="cellIs" dxfId="0" priority="71" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="71" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="cellIs" dxfId="0" priority="73" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="73" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="cellIs" dxfId="0" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="75" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="5" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="cellIs" dxfId="0" priority="77" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="120" priority="77" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="cellIs" dxfId="0" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="79" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="cellIs" dxfId="0" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="81" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="0" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="117" priority="83" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="0" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="85" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="0" priority="87" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="87" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="0" priority="89" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="89" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="cellIs" dxfId="0" priority="91" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="91" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="cellIs" dxfId="0" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="93" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="cellIs" dxfId="0" priority="95" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="95" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="7" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="cellIs" dxfId="0" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="97" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" dxfId="0" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="99" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="cellIs" dxfId="0" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="101" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="cellIs" dxfId="0" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="103" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="cellIs" dxfId="0" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="105" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="cellIs" dxfId="0" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="107" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="cellIs" dxfId="0" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="109" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="0" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="111" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="cellIs" dxfId="0" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="113" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="cellIs" dxfId="0" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="115" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="9" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="cellIs" dxfId="0" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="117" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="cellIs" dxfId="0" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="119" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="cellIs" dxfId="0" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="121" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="cellIs" dxfId="0" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="123" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="cellIs" dxfId="0" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="125" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="cellIs" dxfId="0" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="127" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="cellIs" dxfId="0" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="129" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67">
-    <cfRule type="cellIs" dxfId="0" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="131" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68">
-    <cfRule type="cellIs" dxfId="0" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="133" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69">
-    <cfRule type="cellIs" dxfId="0" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="135" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="11" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="cellIs" dxfId="0" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="137" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71">
-    <cfRule type="cellIs" dxfId="0" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="139" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72">
-    <cfRule type="cellIs" dxfId="0" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="141" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73">
-    <cfRule type="cellIs" dxfId="0" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="143" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74">
-    <cfRule type="cellIs" dxfId="0" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="145" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="cellIs" dxfId="0" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="147" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="cellIs" dxfId="0" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="149" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="cellIs" dxfId="0" priority="151" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="151" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="cellIs" dxfId="0" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="153" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="0" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="13" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="0" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="15" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="0" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="18" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="0" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="20" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="0" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="22" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="0" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="24" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="0" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="26" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="0" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="28" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="0" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="30" operator="greaterThan">
       <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="0" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="32" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="0" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="34" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="0" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="36" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="2" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="cellIs" dxfId="0" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="38" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="0" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="40" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="0" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="42" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="0" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="44" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="0" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="46" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="cellIs" dxfId="0" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="48" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="0" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="50" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="0" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="52" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="0" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="54" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="0" priority="56" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="56" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="4" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="cellIs" dxfId="0" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="58" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="0" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="60" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="0" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="62" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="0" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="64" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="0" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="66" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="0" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="68" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="0" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="70" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="0" priority="72" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="72" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="cellIs" dxfId="0" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="74" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="cellIs" dxfId="0" priority="76" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="76" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="6" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="0" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="78" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="0" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="80" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="0" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="82" operator="greaterThan">
       <formula>22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="0" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="84" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="0" priority="86" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="86" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="cellIs" dxfId="0" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="88" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="0" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="90" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="0" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="92" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="0" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="94" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="0" priority="96" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="96" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="0" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="98" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="0" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="100" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="0" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="102" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="cellIs" dxfId="0" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="104" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="0" priority="106" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="106" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
-    <cfRule type="cellIs" dxfId="0" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="108" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="0" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="110" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="cellIs" dxfId="0" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="112" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="cellIs" dxfId="0" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="114" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="0" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="116" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="0" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="118" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="0" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="120" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="0" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="122" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="0" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="124" operator="greaterThan">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="0" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="126" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="cellIs" dxfId="0" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="128" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="cellIs" dxfId="0" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="130" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="cellIs" dxfId="0" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="132" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="cellIs" dxfId="0" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="134" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="cellIs" dxfId="0" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="136" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="cellIs" dxfId="0" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="138" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="cellIs" dxfId="0" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="140" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72">
-    <cfRule type="cellIs" dxfId="0" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="142" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C73">
-    <cfRule type="cellIs" dxfId="0" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="144" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="0" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="146" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="cellIs" dxfId="0" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="148" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="cellIs" dxfId="0" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="150" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="cellIs" dxfId="0" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="152" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78">
-    <cfRule type="cellIs" dxfId="0" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="154" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="0" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
setting up classes with property decorators
</commit_message>
<xml_diff>
--- a/assets/excel/ping_pong_scoresheet_v2.xlsx
+++ b/assets/excel/ping_pong_scoresheet_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ktuten/Desktop/ping_pong/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14417CC-5C19-5E43-A65E-C5F14EC2B508}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAA9620-8D54-E241-A75E-D50279E0C66C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="15">
   <si>
     <t>Fritz</t>
   </si>
@@ -212,13 +212,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1482,15 +1482,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.3">
@@ -2586,7 +2587,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="10">
+      <c r="A79" s="8">
         <v>43413</v>
       </c>
       <c r="B79" s="1">
@@ -2600,7 +2601,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="10">
+      <c r="A80" s="8">
         <v>43413</v>
       </c>
       <c r="B80" s="1">
@@ -2614,7 +2615,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="10">
+      <c r="A81" s="8">
         <v>43413</v>
       </c>
       <c r="B81" s="1">
@@ -2628,7 +2629,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="10">
+      <c r="A82" s="8">
         <v>43413</v>
       </c>
       <c r="B82" s="1">
@@ -2641,160 +2642,188 @@
         <v>5</v>
       </c>
     </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="8">
+        <v>43417</v>
+      </c>
+      <c r="B83" s="1">
+        <v>15</v>
+      </c>
+      <c r="C83" s="1">
+        <v>13</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C84" s="2" t="s">
+      <c r="A84" s="8">
+        <v>43417</v>
+      </c>
+      <c r="B84" s="1">
+        <v>15</v>
+      </c>
+      <c r="C84" s="1">
+        <v>13</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C86" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="8" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="1">
+      <c r="B87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="1">
         <v>17</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D87" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="9"/>
-      <c r="B86" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C86" s="1">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="10"/>
+      <c r="B88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1">
         <v>20</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D88" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="9"/>
-      <c r="B87" s="2" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="10"/>
+      <c r="B89" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C89" s="1">
         <v>37</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D89" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="9" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="1">
+      <c r="B90" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="1">
         <v>43.59</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D90" s="1">
         <v>47.37</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="9"/>
-      <c r="B89" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C89" s="1">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="10"/>
+      <c r="B91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="1">
         <v>52.63</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D91" s="1">
         <v>56.41</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="9"/>
-      <c r="B90" s="2" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="10"/>
+      <c r="B92" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C92" s="1">
         <v>48.05</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D92" s="1">
         <v>51.95</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="9" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="1">
+      <c r="B93" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="1">
         <v>12.49</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D93" s="1">
         <v>13.92</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="9"/>
-      <c r="B92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C92" s="1">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="10"/>
+      <c r="B94" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C94" s="1">
         <v>13.63</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D94" s="1">
         <v>13.28</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="9"/>
-      <c r="B93" s="2" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="10"/>
+      <c r="B95" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C95" s="1">
         <v>13.05</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D95" s="1">
         <v>13.6</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="9" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C96" s="1">
         <v>1</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D96" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="9"/>
-      <c r="B95" s="2" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="10"/>
+      <c r="B97" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C95" s="1">
-        <v>4</v>
-      </c>
-      <c r="D95" s="1">
+      <c r="C97" s="1">
+        <v>4</v>
+      </c>
+      <c r="D97" s="1">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="A91:A93"/>
-    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A87:A89"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="A93:A95"/>
+    <mergeCell ref="A96:A97"/>
   </mergeCells>
   <conditionalFormatting sqref="B10">
     <cfRule type="cellIs" dxfId="153" priority="17" operator="greaterThan">

</xml_diff>

<commit_message>
formatting for index and stats rows
</commit_message>
<xml_diff>
--- a/assets/excel/ping_pong_scoresheet_v2.xlsx
+++ b/assets/excel/ping_pong_scoresheet_v2.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ktuten/Desktop/ping_pong/assets/excel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A325935D-6142-5F4D-A590-23CEF18B44DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="15">
   <si>
     <t>Fritz</t>
   </si>
@@ -70,11 +64,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,1085 +201,21 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="178">
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -1293,14 +224,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1347,7 +270,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1379,27 +302,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1431,24 +336,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1624,19 +511,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="9.1640625" style="1"/>
+    <col min="1" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1650,7 +535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="4">
         <v>43384</v>
       </c>
@@ -1664,8 +549,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+    <row r="3" spans="1:4">
+      <c r="A3" s="7">
         <v>43384</v>
       </c>
       <c r="B3" s="1">
@@ -1674,11 +559,11 @@
       <c r="C3" s="1">
         <v>15</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="4">
         <v>43384</v>
       </c>
@@ -1692,8 +577,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+    <row r="5" spans="1:4">
+      <c r="A5" s="7">
         <v>43384</v>
       </c>
       <c r="B5" s="1">
@@ -1702,11 +587,11 @@
       <c r="C5" s="1">
         <v>15</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="4">
         <v>43384</v>
       </c>
@@ -1720,8 +605,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+    <row r="7" spans="1:4">
+      <c r="A7" s="7">
         <v>43384</v>
       </c>
       <c r="B7" s="1">
@@ -1730,11 +615,11 @@
       <c r="C7" s="1">
         <v>15</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="4">
         <v>43384</v>
       </c>
@@ -1748,8 +633,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+    <row r="9" spans="1:4">
+      <c r="A9" s="7">
         <v>43384</v>
       </c>
       <c r="B9" s="1">
@@ -1758,11 +643,11 @@
       <c r="C9" s="1">
         <v>15</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="4">
         <v>43384</v>
       </c>
@@ -1776,8 +661,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+    <row r="11" spans="1:4">
+      <c r="A11" s="7">
         <v>43384</v>
       </c>
       <c r="B11" s="1">
@@ -1786,11 +671,11 @@
       <c r="C11" s="1">
         <v>15</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="4">
         <v>43384</v>
       </c>
@@ -1804,8 +689,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+    <row r="13" spans="1:4">
+      <c r="A13" s="7">
         <v>43384</v>
       </c>
       <c r="B13" s="1">
@@ -1814,11 +699,11 @@
       <c r="C13" s="1">
         <v>15</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="4">
         <v>43384</v>
       </c>
@@ -1832,8 +717,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+    <row r="15" spans="1:4">
+      <c r="A15" s="7">
         <v>43384</v>
       </c>
       <c r="B15" s="1">
@@ -1842,11 +727,11 @@
       <c r="C15" s="1">
         <v>15</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="4">
         <v>43384</v>
       </c>
@@ -1860,8 +745,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+    <row r="17" spans="1:4">
+      <c r="A17" s="7">
         <v>43384</v>
       </c>
       <c r="B17" s="1">
@@ -1870,11 +755,11 @@
       <c r="C17" s="1">
         <v>11</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="4">
         <v>43396</v>
       </c>
@@ -1888,8 +773,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+    <row r="19" spans="1:4">
+      <c r="A19" s="7">
         <v>43396</v>
       </c>
       <c r="B19" s="1">
@@ -1898,11 +783,11 @@
       <c r="C19" s="1">
         <v>15</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="4">
         <v>43397</v>
       </c>
@@ -1916,8 +801,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+    <row r="21" spans="1:4">
+      <c r="A21" s="7">
         <v>43397</v>
       </c>
       <c r="B21" s="1">
@@ -1926,11 +811,11 @@
       <c r="C21" s="1">
         <v>10</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="4">
         <v>43397</v>
       </c>
@@ -1944,8 +829,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+    <row r="23" spans="1:4">
+      <c r="A23" s="7">
         <v>43397</v>
       </c>
       <c r="B23" s="1">
@@ -1954,11 +839,11 @@
       <c r="C23" s="1">
         <v>15</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="4">
         <v>43399</v>
       </c>
@@ -1972,8 +857,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+    <row r="25" spans="1:4">
+      <c r="A25" s="7">
         <v>43399</v>
       </c>
       <c r="B25" s="1">
@@ -1982,11 +867,11 @@
       <c r="C25" s="1">
         <v>18</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="4">
         <v>43399</v>
       </c>
@@ -2000,8 +885,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+    <row r="27" spans="1:4">
+      <c r="A27" s="7">
         <v>43399</v>
       </c>
       <c r="B27" s="1">
@@ -2010,11 +895,11 @@
       <c r="C27" s="1">
         <v>13</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="4">
         <v>43399</v>
       </c>
@@ -2028,8 +913,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+    <row r="29" spans="1:4">
+      <c r="A29" s="7">
         <v>43399</v>
       </c>
       <c r="B29" s="1">
@@ -2038,11 +923,11 @@
       <c r="C29" s="1">
         <v>13</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="4">
         <v>43402</v>
       </c>
@@ -2056,8 +941,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
+    <row r="31" spans="1:4">
+      <c r="A31" s="7">
         <v>43402</v>
       </c>
       <c r="B31" s="1">
@@ -2066,11 +951,11 @@
       <c r="C31" s="1">
         <v>12</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="4">
         <v>43402</v>
       </c>
@@ -2084,8 +969,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
+    <row r="33" spans="1:4">
+      <c r="A33" s="7">
         <v>43402</v>
       </c>
       <c r="B33" s="1">
@@ -2094,11 +979,11 @@
       <c r="C33" s="1">
         <v>16</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="4">
         <v>43402</v>
       </c>
@@ -2112,8 +997,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
+    <row r="35" spans="1:4">
+      <c r="A35" s="7">
         <v>43402</v>
       </c>
       <c r="B35" s="1">
@@ -2122,11 +1007,11 @@
       <c r="C35" s="1">
         <v>13</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="4">
         <v>43402</v>
       </c>
@@ -2140,8 +1025,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
+    <row r="37" spans="1:4">
+      <c r="A37" s="7">
         <v>43402</v>
       </c>
       <c r="B37" s="1">
@@ -2150,11 +1035,11 @@
       <c r="C37" s="1">
         <v>15</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="4">
         <v>43402</v>
       </c>
@@ -2168,8 +1053,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
+    <row r="39" spans="1:4">
+      <c r="A39" s="7">
         <v>43402</v>
       </c>
       <c r="B39" s="1">
@@ -2178,11 +1063,11 @@
       <c r="C39" s="1">
         <v>16</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="4">
         <v>43402</v>
       </c>
@@ -2196,8 +1081,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="4">
+    <row r="41" spans="1:4">
+      <c r="A41" s="7">
         <v>43402</v>
       </c>
       <c r="B41" s="1">
@@ -2206,11 +1091,11 @@
       <c r="C41" s="1">
         <v>8</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="4">
         <v>43402</v>
       </c>
@@ -2224,8 +1109,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="4">
+    <row r="43" spans="1:4">
+      <c r="A43" s="7">
         <v>43402</v>
       </c>
       <c r="B43" s="1">
@@ -2234,11 +1119,11 @@
       <c r="C43" s="1">
         <v>13</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="4">
         <v>43402</v>
       </c>
@@ -2252,8 +1137,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="4">
+    <row r="45" spans="1:4">
+      <c r="A45" s="7">
         <v>43402</v>
       </c>
       <c r="B45" s="1">
@@ -2262,11 +1147,11 @@
       <c r="C45" s="1">
         <v>14</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="4">
         <v>43402</v>
       </c>
@@ -2280,8 +1165,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="4">
+    <row r="47" spans="1:4">
+      <c r="A47" s="7">
         <v>43402</v>
       </c>
       <c r="B47" s="1">
@@ -2290,11 +1175,11 @@
       <c r="C47" s="1">
         <v>16</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D47" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="4">
         <v>43402</v>
       </c>
@@ -2308,8 +1193,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
+    <row r="49" spans="1:4">
+      <c r="A49" s="7">
         <v>43405</v>
       </c>
       <c r="B49" s="1">
@@ -2318,11 +1203,11 @@
       <c r="C49" s="1">
         <v>13</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="4">
         <v>43405</v>
       </c>
@@ -2336,8 +1221,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
+    <row r="51" spans="1:4">
+      <c r="A51" s="7">
         <v>43405</v>
       </c>
       <c r="B51" s="1">
@@ -2346,11 +1231,11 @@
       <c r="C51" s="1">
         <v>15</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="4">
         <v>43409</v>
       </c>
@@ -2364,8 +1249,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
+    <row r="53" spans="1:4">
+      <c r="A53" s="7">
         <v>43409</v>
       </c>
       <c r="B53" s="1">
@@ -2374,11 +1259,11 @@
       <c r="C53" s="1">
         <v>7</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D53" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="4">
         <v>43409</v>
       </c>
@@ -2392,8 +1277,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="4">
+    <row r="55" spans="1:4">
+      <c r="A55" s="7">
         <v>43409</v>
       </c>
       <c r="B55" s="1">
@@ -2402,11 +1287,11 @@
       <c r="C55" s="1">
         <v>14</v>
       </c>
-      <c r="D55" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D55" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="4">
         <v>43409</v>
       </c>
@@ -2420,8 +1305,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="4">
+    <row r="57" spans="1:4">
+      <c r="A57" s="7">
         <v>43410</v>
       </c>
       <c r="B57" s="1">
@@ -2430,11 +1315,11 @@
       <c r="C57" s="1">
         <v>15</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D57" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="4">
         <v>43410</v>
       </c>
@@ -2448,8 +1333,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="4">
+    <row r="59" spans="1:4">
+      <c r="A59" s="7">
         <v>43410</v>
       </c>
       <c r="B59" s="1">
@@ -2458,11 +1343,11 @@
       <c r="C59" s="1">
         <v>11</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D59" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="4">
         <v>43410</v>
       </c>
@@ -2476,8 +1361,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="4">
+    <row r="61" spans="1:4">
+      <c r="A61" s="7">
         <v>43410</v>
       </c>
       <c r="B61" s="1">
@@ -2486,11 +1371,11 @@
       <c r="C61" s="1">
         <v>15</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D61" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="4">
         <v>43410</v>
       </c>
@@ -2504,8 +1389,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="4">
+    <row r="63" spans="1:4">
+      <c r="A63" s="7">
         <v>43410</v>
       </c>
       <c r="B63" s="1">
@@ -2514,11 +1399,11 @@
       <c r="C63" s="1">
         <v>15</v>
       </c>
-      <c r="D63" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D63" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="4">
         <v>43410</v>
       </c>
@@ -2532,8 +1417,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="4">
+    <row r="65" spans="1:4">
+      <c r="A65" s="7">
         <v>43410</v>
       </c>
       <c r="B65" s="1">
@@ -2542,11 +1427,11 @@
       <c r="C65" s="1">
         <v>18</v>
       </c>
-      <c r="D65" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D65" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="4">
         <v>43411</v>
       </c>
@@ -2560,8 +1445,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="4">
+    <row r="67" spans="1:4">
+      <c r="A67" s="7">
         <v>43411</v>
       </c>
       <c r="B67" s="1">
@@ -2570,11 +1455,11 @@
       <c r="C67" s="1">
         <v>7</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D67" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="4">
         <v>43411</v>
       </c>
@@ -2588,8 +1473,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="4">
+    <row r="69" spans="1:4">
+      <c r="A69" s="7">
         <v>43411</v>
       </c>
       <c r="B69" s="1">
@@ -2598,11 +1483,11 @@
       <c r="C69" s="1">
         <v>12</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D69" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="4">
         <v>43411</v>
       </c>
@@ -2616,8 +1501,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="4">
+    <row r="71" spans="1:4">
+      <c r="A71" s="7">
         <v>43411</v>
       </c>
       <c r="B71" s="1">
@@ -2626,11 +1511,11 @@
       <c r="C71" s="1">
         <v>15</v>
       </c>
-      <c r="D71" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D71" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="4">
         <v>43411</v>
       </c>
@@ -2644,8 +1529,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="4">
+    <row r="73" spans="1:4">
+      <c r="A73" s="7">
         <v>43412</v>
       </c>
       <c r="B73" s="1">
@@ -2654,11 +1539,11 @@
       <c r="C73" s="1">
         <v>14</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D73" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="4">
         <v>43412</v>
       </c>
@@ -2672,8 +1557,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="4">
+    <row r="75" spans="1:4">
+      <c r="A75" s="7">
         <v>43412</v>
       </c>
       <c r="B75" s="1">
@@ -2682,11 +1567,11 @@
       <c r="C75" s="1">
         <v>3</v>
       </c>
-      <c r="D75" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D75" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="4">
         <v>43412</v>
       </c>
@@ -2700,8 +1585,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="4">
+    <row r="77" spans="1:4">
+      <c r="A77" s="7">
         <v>43412</v>
       </c>
       <c r="B77" s="1">
@@ -2710,11 +1595,11 @@
       <c r="C77" s="1">
         <v>15</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D77" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="4">
         <v>43412</v>
       </c>
@@ -2728,8 +1613,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="4">
+    <row r="79" spans="1:4">
+      <c r="A79" s="7">
         <v>43413</v>
       </c>
       <c r="B79" s="1">
@@ -2738,11 +1623,11 @@
       <c r="C79" s="1">
         <v>12</v>
       </c>
-      <c r="D79" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D79" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="4">
         <v>43413</v>
       </c>
@@ -2756,8 +1641,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="4">
+    <row r="81" spans="1:4">
+      <c r="A81" s="7">
         <v>43413</v>
       </c>
       <c r="B81" s="1">
@@ -2766,11 +1651,11 @@
       <c r="C81" s="1">
         <v>16</v>
       </c>
-      <c r="D81" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D81" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="4">
         <v>43413</v>
       </c>
@@ -2784,8 +1669,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="4">
+    <row r="83" spans="1:4">
+      <c r="A83" s="7">
         <v>43417</v>
       </c>
       <c r="B83" s="1">
@@ -2794,11 +1679,11 @@
       <c r="C83" s="1">
         <v>13</v>
       </c>
-      <c r="D83" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D83" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="4">
         <v>43417</v>
       </c>
@@ -2812,8 +1697,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="4">
+    <row r="85" spans="1:4">
+      <c r="A85" s="7">
         <v>43417</v>
       </c>
       <c r="B85" s="1">
@@ -2822,11 +1707,11 @@
       <c r="C85" s="1">
         <v>7</v>
       </c>
-      <c r="D85" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D85" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="4">
         <v>43417</v>
       </c>
@@ -2840,8 +1725,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="4">
+    <row r="87" spans="1:4">
+      <c r="A87" s="7">
         <v>43418</v>
       </c>
       <c r="B87" s="1">
@@ -2850,11 +1735,11 @@
       <c r="C87" s="1">
         <v>12</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D87" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="4">
         <v>43418</v>
       </c>
@@ -2868,8 +1753,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="4">
+    <row r="89" spans="1:4">
+      <c r="A89" s="7">
         <v>43418</v>
       </c>
       <c r="B89" s="1">
@@ -2878,11 +1763,11 @@
       <c r="C89" s="1">
         <v>11</v>
       </c>
-      <c r="D89" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D89" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="4">
         <v>43418</v>
       </c>
@@ -2896,7 +1781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4">
       <c r="C92" s="2" t="s">
         <v>6</v>
       </c>
@@ -2904,34 +1789,34 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="8" t="s">
+    <row r="93" spans="1:4">
+      <c r="A93" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C93" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D93" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="9"/>
+    <row r="94" spans="1:4">
+      <c r="A94" s="2"/>
       <c r="B94" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C94" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D94" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="9"/>
+    <row r="95" spans="1:4">
+      <c r="A95" s="2"/>
       <c r="B95" s="2" t="s">
         <v>12</v>
       </c>
@@ -2942,34 +1827,34 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="9" t="s">
+    <row r="96" spans="1:4">
+      <c r="A96" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C96" s="1">
-        <v>50</v>
+        <v>48.89</v>
       </c>
       <c r="D96" s="1">
-        <v>44.19</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="9"/>
+        <v>43.18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="2"/>
       <c r="B97" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C97" s="1">
-        <v>55.81</v>
+        <v>56.82</v>
       </c>
       <c r="D97" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="9"/>
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="2"/>
       <c r="B98" s="2" t="s">
         <v>12</v>
       </c>
@@ -2980,34 +1865,34 @@
         <v>47.19</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="9" t="s">
+    <row r="99" spans="1:4">
+      <c r="A99" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C99" s="1">
-        <v>12.91</v>
+        <v>12.87</v>
       </c>
       <c r="D99" s="1">
-        <v>13.77</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="9"/>
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="2"/>
       <c r="B100" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C100" s="1">
-        <v>13.77</v>
+        <v>13.8</v>
       </c>
       <c r="D100" s="1">
-        <v>13.2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="9"/>
+        <v>13.24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="2"/>
       <c r="B101" s="2" t="s">
         <v>12</v>
       </c>
@@ -3018,8 +1903,8 @@
         <v>13.47</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="9" t="s">
+    <row r="102" spans="1:4">
+      <c r="A102" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -3032,8 +1917,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="9"/>
+    <row r="103" spans="1:4">
+      <c r="A103" s="2"/>
       <c r="B103" s="2" t="s">
         <v>14</v>
       </c>
@@ -3052,887 +1937,887 @@
     <mergeCell ref="A102:A103"/>
   </mergeCells>
   <conditionalFormatting sqref="B10">
-    <cfRule type="cellIs" dxfId="177" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="cellIs" dxfId="176" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="19" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="175" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="174" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="23" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="173" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="25" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="cellIs" dxfId="172" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="27" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="cellIs" dxfId="171" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="29" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="cellIs" dxfId="170" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="31" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="cellIs" dxfId="169" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="33" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="168" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="35" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="167" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="166" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="37" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="165" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="39" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="cellIs" dxfId="164" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="41" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="cellIs" dxfId="163" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="43" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="162" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="45" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="cellIs" dxfId="161" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="47" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="cellIs" dxfId="160" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="49" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="159" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="51" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="158" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="53" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="157" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="55" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="156" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="155" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="57" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="cellIs" dxfId="154" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="59" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="153" priority="61" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="61" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="cellIs" dxfId="152" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="63" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="cellIs" dxfId="151" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="65" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="cellIs" dxfId="150" priority="67" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="67" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="149" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="69" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="cellIs" dxfId="148" priority="71" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="71" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="cellIs" dxfId="147" priority="73" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="73" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="cellIs" dxfId="146" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="75" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="145" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="cellIs" dxfId="144" priority="77" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="77" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="cellIs" dxfId="143" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="79" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="cellIs" dxfId="142" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="81" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="141" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="83" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="140" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="85" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="139" priority="87" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="87" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="138" priority="89" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="89" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="cellIs" dxfId="137" priority="91" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="91" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="cellIs" dxfId="136" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="93" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="cellIs" dxfId="135" priority="95" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="95" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="134" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="cellIs" dxfId="133" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="97" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" dxfId="132" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="99" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="cellIs" dxfId="131" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="101" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="cellIs" dxfId="130" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="103" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="cellIs" dxfId="129" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="105" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="cellIs" dxfId="128" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="107" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="cellIs" dxfId="127" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="109" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="126" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="111" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="cellIs" dxfId="125" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="113" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="cellIs" dxfId="124" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="115" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="123" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="cellIs" dxfId="122" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="117" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="cellIs" dxfId="121" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="119" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="cellIs" dxfId="120" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="121" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="cellIs" dxfId="119" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="123" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="cellIs" dxfId="118" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="125" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="cellIs" dxfId="117" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="127" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="cellIs" dxfId="116" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="129" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67">
-    <cfRule type="cellIs" dxfId="115" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="131" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68">
-    <cfRule type="cellIs" dxfId="114" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="133" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69">
-    <cfRule type="cellIs" dxfId="113" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="135" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="112" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="cellIs" dxfId="111" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="137" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71">
-    <cfRule type="cellIs" dxfId="110" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="139" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72">
-    <cfRule type="cellIs" dxfId="109" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="141" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73">
-    <cfRule type="cellIs" dxfId="108" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="143" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74">
-    <cfRule type="cellIs" dxfId="107" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="145" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="cellIs" dxfId="106" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="147" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="cellIs" dxfId="105" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="149" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="cellIs" dxfId="104" priority="151" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="151" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="cellIs" dxfId="103" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="153" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="cellIs" dxfId="102" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="155" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="101" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80">
-    <cfRule type="cellIs" dxfId="100" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="157" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81">
-    <cfRule type="cellIs" dxfId="99" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="159" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82">
-    <cfRule type="cellIs" dxfId="98" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="161" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="cellIs" dxfId="97" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="163" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="cellIs" dxfId="96" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="165" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85">
-    <cfRule type="cellIs" dxfId="95" priority="167" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="167" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="cellIs" dxfId="94" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="169" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="cellIs" dxfId="93" priority="171" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="171" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="cellIs" dxfId="92" priority="173" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="173" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="cellIs" dxfId="91" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="175" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="90" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="cellIs" dxfId="89" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="177" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="88" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="87" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="20" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="86" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="22" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="85" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="24" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="84" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="26" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="83" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="28" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="82" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="30" operator="greaterThan">
       <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="81" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="32" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="80" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="34" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="79" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="36" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="78" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="cellIs" dxfId="77" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="38" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="76" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="40" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="75" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="42" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="74" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="44" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="73" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="46" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="cellIs" dxfId="72" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="48" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="71" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="50" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="70" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="52" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="69" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="54" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="68" priority="56" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="56" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="67" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="cellIs" dxfId="66" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="58" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="65" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="60" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="64" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="62" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="64" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="62" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="66" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="61" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="68" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="60" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="70" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="59" priority="72" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="72" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="cellIs" dxfId="58" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="74" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="cellIs" dxfId="57" priority="76" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="76" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="56" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="55" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="78" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="54" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="80" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="53" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="82" operator="greaterThan">
       <formula>22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="52" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="84" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="51" priority="86" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="86" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="cellIs" dxfId="50" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="88" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="49" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="90" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="48" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="92" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="47" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="94" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="46" priority="96" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="96" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="45" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="44" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="98" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="43" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="100" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="42" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="102" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="cellIs" dxfId="41" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="104" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="40" priority="106" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="106" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
-    <cfRule type="cellIs" dxfId="39" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="108" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="38" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="110" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="cellIs" dxfId="37" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="112" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="cellIs" dxfId="36" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="114" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="35" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="116" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="33" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="118" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="32" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="120" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="31" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="122" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="30" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="124" operator="greaterThan">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="29" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="126" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="cellIs" dxfId="28" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="128" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="cellIs" dxfId="27" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="130" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="cellIs" dxfId="26" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="132" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="cellIs" dxfId="25" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="134" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="cellIs" dxfId="24" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="136" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="23" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="cellIs" dxfId="22" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="138" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="cellIs" dxfId="21" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="140" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72">
-    <cfRule type="cellIs" dxfId="20" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="142" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C73">
-    <cfRule type="cellIs" dxfId="19" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="144" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="18" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="146" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="cellIs" dxfId="17" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="148" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="cellIs" dxfId="16" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="150" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="cellIs" dxfId="15" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="152" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78">
-    <cfRule type="cellIs" dxfId="14" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="154" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79">
-    <cfRule type="cellIs" dxfId="13" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="156" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80">
-    <cfRule type="cellIs" dxfId="11" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="158" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81">
-    <cfRule type="cellIs" dxfId="10" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="160" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82">
-    <cfRule type="cellIs" dxfId="9" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="162" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="cellIs" dxfId="8" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="164" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84">
-    <cfRule type="cellIs" dxfId="7" priority="166" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="166" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="cellIs" dxfId="6" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="168" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="cellIs" dxfId="5" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="170" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="cellIs" dxfId="4" priority="172" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="172" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88">
-    <cfRule type="cellIs" dxfId="3" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="174" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="cellIs" dxfId="2" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="176" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="1" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
consolidated dictionaries and workbook formatting
</commit_message>
<xml_diff>
--- a/assets/excel/ping_pong_scoresheet_v2.xlsx
+++ b/assets/excel/ping_pong_scoresheet_v2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="15">
   <si>
     <t>Fritz</t>
   </si>
@@ -65,8 +65,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="5">
@@ -76,12 +77,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -102,7 +97,13 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Helvetica Neue"/>
+      <name val="AppleGothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="AppleGothic"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -126,7 +127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -173,42 +174,34 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC9C9C9"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFC9C9C9"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC9C9C9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC9C9C9"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -512,1429 +505,1482 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="5" width="9.140625" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>43384</v>
       </c>
-      <c r="B2" s="5">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="4">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>43384</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="C3" s="1">
-        <v>15</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>43384</v>
       </c>
-      <c r="B4" s="5">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="4">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>43384</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" s="1">
-        <v>15</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>43384</v>
       </c>
-      <c r="B6" s="5">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="4">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>43384</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>10</v>
       </c>
-      <c r="C7" s="1">
-        <v>15</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>43384</v>
       </c>
-      <c r="B8" s="5">
-        <v>15</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="4">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4">
         <v>10</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>43384</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>10</v>
       </c>
-      <c r="C9" s="1">
-        <v>15</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>43384</v>
       </c>
-      <c r="B10" s="5">
-        <v>15</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="4">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4">
         <v>10</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>43384</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" s="1">
-        <v>15</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>43384</v>
       </c>
-      <c r="B12" s="5">
-        <v>15</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B12" s="4">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4">
         <v>10</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>43384</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>10</v>
       </c>
-      <c r="C13" s="1">
-        <v>15</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>43384</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="5">
-        <v>15</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="4">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>43384</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>7</v>
       </c>
-      <c r="C15" s="1">
-        <v>15</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>43384</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>17</v>
       </c>
-      <c r="C16" s="5">
-        <v>15</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="4">
+        <v>15</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>43384</v>
       </c>
-      <c r="B17" s="1">
-        <v>15</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
         <v>11</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>43396</v>
       </c>
-      <c r="B18" s="5">
-        <v>15</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="B18" s="4">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4">
         <v>12</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <v>43396</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>9</v>
       </c>
-      <c r="C19" s="1">
-        <v>15</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>43397</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>11</v>
       </c>
-      <c r="C20" s="5">
-        <v>15</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="4">
+        <v>15</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>43397</v>
       </c>
-      <c r="B21" s="1">
-        <v>15</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21">
         <v>10</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>43397</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>20</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>18</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>43397</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
         <v>7</v>
       </c>
-      <c r="C23" s="1">
-        <v>15</v>
-      </c>
-      <c r="D23" s="8" t="s">
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>43399</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>13</v>
       </c>
-      <c r="C24" s="5">
-        <v>15</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="4">
+        <v>15</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>43399</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>20</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>18</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>43399</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>12</v>
       </c>
-      <c r="C26" s="5">
-        <v>15</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="C26" s="4">
+        <v>15</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="7">
+      <c r="A27" s="6">
         <v>43399</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>11</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>13</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>43399</v>
       </c>
-      <c r="B28" s="5">
-        <v>15</v>
-      </c>
-      <c r="C28" s="5">
+      <c r="B28" s="4">
+        <v>15</v>
+      </c>
+      <c r="C28" s="4">
         <v>11</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>43399</v>
       </c>
-      <c r="B29" s="1">
-        <v>15</v>
-      </c>
-      <c r="C29" s="1">
+      <c r="B29">
+        <v>15</v>
+      </c>
+      <c r="C29">
         <v>13</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>43402</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>12</v>
       </c>
-      <c r="C30" s="5">
-        <v>15</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="C30" s="4">
+        <v>15</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="7">
+      <c r="A31" s="6">
         <v>43402</v>
       </c>
-      <c r="B31" s="1">
-        <v>15</v>
-      </c>
-      <c r="C31" s="1">
+      <c r="B31">
+        <v>15</v>
+      </c>
+      <c r="C31">
         <v>12</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>43402</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>16</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>14</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="7">
+      <c r="A33" s="6">
         <v>43402</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
         <v>18</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>16</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>43402</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>8</v>
       </c>
-      <c r="C34" s="5">
-        <v>15</v>
-      </c>
-      <c r="D34" s="6" t="s">
+      <c r="C34" s="4">
+        <v>15</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>43402</v>
       </c>
-      <c r="B35" s="1">
-        <v>15</v>
-      </c>
-      <c r="C35" s="1">
+      <c r="B35">
+        <v>15</v>
+      </c>
+      <c r="C35">
         <v>13</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>43402</v>
       </c>
-      <c r="B36" s="5">
-        <v>15</v>
-      </c>
-      <c r="C36" s="5">
+      <c r="B36" s="4">
+        <v>15</v>
+      </c>
+      <c r="C36" s="4">
         <v>11</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="7">
+      <c r="A37" s="6">
         <v>43402</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37">
         <v>12</v>
       </c>
-      <c r="C37" s="1">
-        <v>15</v>
-      </c>
-      <c r="D37" s="8" t="s">
+      <c r="C37">
+        <v>15</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>43402</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="4">
         <v>13</v>
       </c>
-      <c r="C38" s="5">
-        <v>15</v>
-      </c>
-      <c r="D38" s="6" t="s">
+      <c r="C38" s="4">
+        <v>15</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="7">
+      <c r="A39" s="6">
         <v>43402</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39">
         <v>14</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39">
         <v>16</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>43402</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="4">
         <v>9</v>
       </c>
-      <c r="C40" s="5">
-        <v>15</v>
-      </c>
-      <c r="D40" s="6" t="s">
+      <c r="C40" s="4">
+        <v>15</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="7">
+      <c r="A41" s="6">
         <v>43402</v>
       </c>
-      <c r="B41" s="1">
-        <v>15</v>
-      </c>
-      <c r="C41" s="1">
+      <c r="B41">
+        <v>15</v>
+      </c>
+      <c r="C41">
         <v>8</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>43402</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="4">
         <v>22</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <v>20</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="7">
+      <c r="A43" s="6">
         <v>43402</v>
       </c>
-      <c r="B43" s="1">
-        <v>15</v>
-      </c>
-      <c r="C43" s="1">
+      <c r="B43">
+        <v>15</v>
+      </c>
+      <c r="C43">
         <v>13</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>43402</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="4">
         <v>9</v>
       </c>
-      <c r="C44" s="5">
-        <v>15</v>
-      </c>
-      <c r="D44" s="6" t="s">
+      <c r="C44" s="4">
+        <v>15</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="7">
+      <c r="A45" s="6">
         <v>43402</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45">
         <v>16</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45">
         <v>14</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>43402</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="4">
         <v>14</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="4">
         <v>16</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="7">
+      <c r="A47" s="6">
         <v>43402</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47">
         <v>14</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47">
         <v>16</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>43402</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="4">
         <v>16</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="4">
         <v>18</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="7">
+      <c r="A49" s="6">
         <v>43405</v>
       </c>
-      <c r="B49" s="1">
-        <v>15</v>
-      </c>
-      <c r="C49" s="1">
+      <c r="B49">
+        <v>15</v>
+      </c>
+      <c r="C49">
         <v>13</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>43405</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="4">
         <v>11</v>
       </c>
-      <c r="C50" s="5">
-        <v>15</v>
-      </c>
-      <c r="D50" s="6" t="s">
+      <c r="C50" s="4">
+        <v>15</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="7">
+      <c r="A51" s="6">
         <v>43405</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51">
         <v>10</v>
       </c>
-      <c r="C51" s="1">
-        <v>15</v>
-      </c>
-      <c r="D51" s="8" t="s">
+      <c r="C51">
+        <v>15</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>43409</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="4">
         <v>12</v>
       </c>
-      <c r="C52" s="5">
-        <v>15</v>
-      </c>
-      <c r="D52" s="6" t="s">
+      <c r="C52" s="4">
+        <v>15</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="7">
+      <c r="A53" s="6">
         <v>43409</v>
       </c>
-      <c r="B53" s="1">
-        <v>15</v>
-      </c>
-      <c r="C53" s="1">
+      <c r="B53">
+        <v>15</v>
+      </c>
+      <c r="C53">
         <v>7</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>43409</v>
       </c>
-      <c r="B54" s="5">
-        <v>15</v>
-      </c>
-      <c r="C54" s="5">
+      <c r="B54" s="4">
+        <v>15</v>
+      </c>
+      <c r="C54" s="4">
         <v>7</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="7">
+      <c r="A55" s="6">
         <v>43409</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55">
         <v>16</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55">
         <v>14</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>43409</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56" s="4">
         <v>8</v>
       </c>
-      <c r="C56" s="5">
-        <v>15</v>
-      </c>
-      <c r="D56" s="6" t="s">
+      <c r="C56" s="4">
+        <v>15</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="7">
+      <c r="A57" s="6">
         <v>43410</v>
       </c>
-      <c r="B57" s="1">
-        <v>5</v>
-      </c>
-      <c r="C57" s="1">
-        <v>15</v>
-      </c>
-      <c r="D57" s="8" t="s">
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>15</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>43410</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="4">
         <v>11</v>
       </c>
-      <c r="C58" s="5">
-        <v>15</v>
-      </c>
-      <c r="D58" s="6" t="s">
+      <c r="C58" s="4">
+        <v>15</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="7">
+      <c r="A59" s="6">
         <v>43410</v>
       </c>
-      <c r="B59" s="1">
-        <v>15</v>
-      </c>
-      <c r="C59" s="1">
+      <c r="B59">
+        <v>15</v>
+      </c>
+      <c r="C59">
         <v>11</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="4">
+      <c r="A60" s="3">
         <v>43410</v>
       </c>
-      <c r="B60" s="5">
-        <v>15</v>
-      </c>
-      <c r="C60" s="5">
+      <c r="B60" s="4">
+        <v>15</v>
+      </c>
+      <c r="C60" s="4">
         <v>9</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="7">
+      <c r="A61" s="6">
         <v>43410</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61">
         <v>10</v>
       </c>
-      <c r="C61" s="1">
-        <v>15</v>
-      </c>
-      <c r="D61" s="8" t="s">
+      <c r="C61">
+        <v>15</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>43410</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B62" s="4">
         <v>9</v>
       </c>
-      <c r="C62" s="5">
-        <v>15</v>
-      </c>
-      <c r="D62" s="6" t="s">
+      <c r="C62" s="4">
+        <v>15</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="7">
+      <c r="A63" s="6">
         <v>43410</v>
       </c>
-      <c r="B63" s="1">
-        <v>4</v>
-      </c>
-      <c r="C63" s="1">
-        <v>15</v>
-      </c>
-      <c r="D63" s="8" t="s">
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>15</v>
+      </c>
+      <c r="D63" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="4">
+      <c r="A64" s="3">
         <v>43410</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="4">
         <v>14</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64" s="4">
         <v>16</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D64" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="7">
+      <c r="A65" s="6">
         <v>43410</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65">
         <v>16</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65">
         <v>18</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="D65" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="4">
+      <c r="A66" s="3">
         <v>43411</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B66" s="4">
         <v>9</v>
       </c>
-      <c r="C66" s="5">
-        <v>15</v>
-      </c>
-      <c r="D66" s="6" t="s">
+      <c r="C66" s="4">
+        <v>15</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="7">
+      <c r="A67" s="6">
         <v>43411</v>
       </c>
-      <c r="B67" s="1">
-        <v>15</v>
-      </c>
-      <c r="C67" s="1">
+      <c r="B67">
+        <v>15</v>
+      </c>
+      <c r="C67">
         <v>7</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="D67" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="4">
+      <c r="A68" s="3">
         <v>43411</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B68" s="4">
         <v>16</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C68" s="4">
         <v>14</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="7">
+      <c r="A69" s="6">
         <v>43411</v>
       </c>
-      <c r="B69" s="1">
-        <v>15</v>
-      </c>
-      <c r="C69" s="1">
+      <c r="B69">
+        <v>15</v>
+      </c>
+      <c r="C69">
         <v>12</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="D69" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="4">
+      <c r="A70" s="3">
         <v>43411</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B70" s="4">
         <v>12</v>
       </c>
-      <c r="C70" s="5">
-        <v>15</v>
-      </c>
-      <c r="D70" s="6" t="s">
+      <c r="C70" s="4">
+        <v>15</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="7">
+      <c r="A71" s="6">
         <v>43411</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71">
         <v>12</v>
       </c>
-      <c r="C71" s="1">
-        <v>15</v>
-      </c>
-      <c r="D71" s="8" t="s">
+      <c r="C71">
+        <v>15</v>
+      </c>
+      <c r="D71" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="4">
+      <c r="A72" s="3">
         <v>43411</v>
       </c>
-      <c r="B72" s="5">
+      <c r="B72" s="4">
         <v>18</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C72" s="4">
         <v>16</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="D72" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="7">
+      <c r="A73" s="6">
         <v>43412</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73">
         <v>16</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73">
         <v>14</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D73" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="4">
+      <c r="A74" s="3">
         <v>43412</v>
       </c>
-      <c r="B74" s="5">
-        <v>15</v>
-      </c>
-      <c r="C74" s="5">
+      <c r="B74" s="4">
+        <v>15</v>
+      </c>
+      <c r="C74" s="4">
         <v>11</v>
       </c>
-      <c r="D74" s="6" t="s">
+      <c r="D74" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="7">
+      <c r="A75" s="6">
         <v>43412</v>
       </c>
-      <c r="B75" s="1">
-        <v>15</v>
-      </c>
-      <c r="C75" s="1">
+      <c r="B75">
+        <v>15</v>
+      </c>
+      <c r="C75">
         <v>3</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="4">
+      <c r="A76" s="3">
         <v>43412</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="4">
         <v>9</v>
       </c>
-      <c r="C76" s="5">
-        <v>15</v>
-      </c>
-      <c r="D76" s="6" t="s">
+      <c r="C76" s="4">
+        <v>15</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="7">
+      <c r="A77" s="6">
         <v>43412</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77">
         <v>7</v>
       </c>
-      <c r="C77" s="1">
-        <v>15</v>
-      </c>
-      <c r="D77" s="8" t="s">
+      <c r="C77">
+        <v>15</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="4">
+      <c r="A78" s="3">
         <v>43412</v>
       </c>
-      <c r="B78" s="5">
-        <v>15</v>
-      </c>
-      <c r="C78" s="5">
+      <c r="B78" s="4">
+        <v>15</v>
+      </c>
+      <c r="C78" s="4">
         <v>12</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="D78" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="7">
+      <c r="A79" s="6">
         <v>43413</v>
       </c>
-      <c r="B79" s="1">
-        <v>15</v>
-      </c>
-      <c r="C79" s="1">
+      <c r="B79">
+        <v>15</v>
+      </c>
+      <c r="C79">
         <v>12</v>
       </c>
-      <c r="D79" s="8" t="s">
+      <c r="D79" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="4">
+      <c r="A80" s="3">
         <v>43413</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B80" s="4">
         <v>16</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C80" s="4">
         <v>18</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D80" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="7">
+      <c r="A81" s="6">
         <v>43413</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81">
         <v>18</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81">
         <v>16</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D81" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="4">
+      <c r="A82" s="3">
         <v>43413</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82" s="4">
         <v>16</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C82" s="4">
         <v>14</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D82" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="7">
+      <c r="A83" s="6">
         <v>43417</v>
       </c>
-      <c r="B83" s="1">
-        <v>15</v>
-      </c>
-      <c r="C83" s="1">
+      <c r="B83">
+        <v>15</v>
+      </c>
+      <c r="C83">
         <v>13</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D83" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="4">
+      <c r="A84" s="3">
         <v>43417</v>
       </c>
-      <c r="B84" s="5">
-        <v>15</v>
-      </c>
-      <c r="C84" s="5">
+      <c r="B84" s="4">
+        <v>15</v>
+      </c>
+      <c r="C84" s="4">
         <v>13</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="D84" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="7">
+      <c r="A85" s="6">
         <v>43417</v>
       </c>
-      <c r="B85" s="1">
-        <v>15</v>
-      </c>
-      <c r="C85" s="1">
+      <c r="B85">
+        <v>15</v>
+      </c>
+      <c r="C85">
         <v>7</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="D85" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="4">
+      <c r="A86" s="3">
         <v>43417</v>
       </c>
-      <c r="B86" s="5">
+      <c r="B86" s="4">
         <v>11</v>
       </c>
-      <c r="C86" s="5">
-        <v>15</v>
-      </c>
-      <c r="D86" s="6" t="s">
+      <c r="C86" s="4">
+        <v>15</v>
+      </c>
+      <c r="D86" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="7">
+      <c r="A87" s="6">
         <v>43418</v>
       </c>
-      <c r="B87" s="1">
-        <v>15</v>
-      </c>
-      <c r="C87" s="1">
+      <c r="B87">
+        <v>15</v>
+      </c>
+      <c r="C87">
         <v>12</v>
       </c>
-      <c r="D87" s="8" t="s">
+      <c r="D87" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="4">
+      <c r="A88" s="3">
         <v>43418</v>
       </c>
-      <c r="B88" s="5">
-        <v>15</v>
-      </c>
-      <c r="C88" s="5">
+      <c r="B88" s="4">
+        <v>15</v>
+      </c>
+      <c r="C88" s="4">
         <v>11</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="D88" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="7">
+      <c r="A89" s="6">
         <v>43418</v>
       </c>
-      <c r="B89" s="1">
-        <v>15</v>
-      </c>
-      <c r="C89" s="1">
+      <c r="B89">
+        <v>15</v>
+      </c>
+      <c r="C89">
         <v>11</v>
       </c>
-      <c r="D89" s="8" t="s">
+      <c r="D89" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="4">
+      <c r="A90" s="3">
         <v>43418</v>
       </c>
-      <c r="B90" s="5">
-        <v>15</v>
-      </c>
-      <c r="C90" s="5">
+      <c r="B90" s="4">
+        <v>15</v>
+      </c>
+      <c r="C90" s="4">
         <v>10</v>
       </c>
-      <c r="D90" s="6" t="s">
-        <v>5</v>
+      <c r="D90" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="6">
+        <v>43419</v>
+      </c>
+      <c r="B91">
+        <v>10</v>
+      </c>
+      <c r="C91">
+        <v>15</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:4">
-      <c r="C92" s="2" t="s">
+      <c r="A92" s="3">
+        <v>43419</v>
+      </c>
+      <c r="B92" s="4">
+        <v>15</v>
+      </c>
+      <c r="C92" s="4">
+        <v>10</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="6">
+        <v>43419</v>
+      </c>
+      <c r="B93">
+        <v>12</v>
+      </c>
+      <c r="C93">
+        <v>15</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="3">
+        <v>43419</v>
+      </c>
+      <c r="B94" s="4">
+        <v>15</v>
+      </c>
+      <c r="C94" s="4">
+        <v>17</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="C96" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D96" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="9" t="s">
+    <row r="97" spans="1:4">
+      <c r="A97" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="1">
+      <c r="B97" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97">
         <v>22</v>
       </c>
-      <c r="D93" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C94" s="1">
+      <c r="D97">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98">
+        <v>26</v>
+      </c>
+      <c r="D98">
         <v>25</v>
       </c>
-      <c r="D94" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2" t="s">
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C95" s="1">
-        <v>47</v>
-      </c>
-      <c r="D95" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="2" t="s">
+      <c r="C99">
+        <v>48</v>
+      </c>
+      <c r="D99">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" s="1">
-        <v>48.89</v>
-      </c>
-      <c r="D96" s="1">
-        <v>43.18</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="2"/>
-      <c r="B97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C97" s="1">
-        <v>56.82</v>
-      </c>
-      <c r="D97" s="1">
-        <v>51.11</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2" t="s">
+      <c r="B100" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100">
+        <v>46.81</v>
+      </c>
+      <c r="D100">
+        <v>43.48</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C101">
+        <v>56.52</v>
+      </c>
+      <c r="D101">
+        <v>53.19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C98" s="1">
-        <v>52.81</v>
-      </c>
-      <c r="D98" s="1">
-        <v>47.19</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="2" t="s">
+      <c r="C102">
+        <v>51.61</v>
+      </c>
+      <c r="D102">
+        <v>48.39</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="1">
-        <v>12.87</v>
-      </c>
-      <c r="D99" s="1">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C100" s="1">
-        <v>13.8</v>
-      </c>
-      <c r="D100" s="1">
-        <v>13.24</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="2"/>
-      <c r="B101" s="2" t="s">
+      <c r="B103" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103">
+        <v>12.85</v>
+      </c>
+      <c r="D103">
+        <v>13.65</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C104">
+        <v>13.78</v>
+      </c>
+      <c r="D104">
+        <v>13.36</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C101" s="1">
-        <v>13.33</v>
-      </c>
-      <c r="D101" s="1">
-        <v>13.47</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="2" t="s">
+      <c r="C105">
+        <v>13.31</v>
+      </c>
+      <c r="D105">
+        <v>13.51</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B106" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C102" s="1">
-        <v>4</v>
-      </c>
-      <c r="D102" s="1">
+      <c r="C106">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="2"/>
-      <c r="B103" s="2" t="s">
+      <c r="D106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C103" s="1">
-        <v>5</v>
-      </c>
-      <c r="D103" s="1">
+      <c r="C107">
+        <v>5</v>
+      </c>
+      <c r="D107">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A93:A95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="A106:A107"/>
   </mergeCells>
   <conditionalFormatting sqref="B10">
     <cfRule type="cellIs" dxfId="0" priority="17" operator="greaterThan">
@@ -2381,6 +2427,26 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B91">
+    <cfRule type="cellIs" dxfId="0" priority="179" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B92">
+    <cfRule type="cellIs" dxfId="0" priority="181" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B93">
+    <cfRule type="cellIs" dxfId="0" priority="183" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B94">
+    <cfRule type="cellIs" dxfId="0" priority="185" operator="greaterThan">
+      <formula>17</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C10">
     <cfRule type="cellIs" dxfId="0" priority="18" operator="greaterThan">
       <formula>15</formula>
@@ -2826,6 +2892,26 @@
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C91">
+    <cfRule type="cellIs" dxfId="0" priority="180" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C92">
+    <cfRule type="cellIs" dxfId="0" priority="182" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C93">
+    <cfRule type="cellIs" dxfId="0" priority="184" operator="greaterThan">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C94">
+    <cfRule type="cellIs" dxfId="0" priority="186" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed old versions, small formatting change
</commit_message>
<xml_diff>
--- a/assets/excel/ping_pong_scoresheet_v2.xlsx
+++ b/assets/excel/ping_pong_scoresheet_v2.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ktuten/Desktop/ping_pong/assets/excel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A301DD9A-72BC-6443-8C00-BE81327E7A17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="15">
   <si>
     <t>Fritz</t>
   </si>
@@ -70,12 +64,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,8 +111,9 @@
       <b/>
       <sz val="13"/>
       <color rgb="FF000000"/>
-      <name val="AppleGothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -249,7 +254,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -258,7 +263,7 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -267,23 +272,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -291,1415 +284,29 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="234">
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -1708,14 +315,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1762,7 +361,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1794,27 +393,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1846,24 +427,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2039,19 +602,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D131"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119:XFD119"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2065,7 +626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>43384</v>
       </c>
@@ -2079,7 +640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="5">
         <v>43384</v>
       </c>
@@ -2093,7 +654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>43384</v>
       </c>
@@ -2107,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="5">
         <v>43384</v>
       </c>
@@ -2121,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2">
         <v>43384</v>
       </c>
@@ -2135,7 +696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="5">
         <v>43384</v>
       </c>
@@ -2149,7 +710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="2">
         <v>43384</v>
       </c>
@@ -2163,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="5">
         <v>43384</v>
       </c>
@@ -2177,7 +738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>43384</v>
       </c>
@@ -2191,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="5">
         <v>43384</v>
       </c>
@@ -2205,7 +766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="2">
         <v>43384</v>
       </c>
@@ -2219,7 +780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="5">
         <v>43384</v>
       </c>
@@ -2233,7 +794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="2">
         <v>43384</v>
       </c>
@@ -2247,7 +808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="5">
         <v>43384</v>
       </c>
@@ -2261,7 +822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="2">
         <v>43384</v>
       </c>
@@ -2275,7 +836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="5">
         <v>43384</v>
       </c>
@@ -2289,7 +850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="2">
         <v>43396</v>
       </c>
@@ -2303,7 +864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="5">
         <v>43396</v>
       </c>
@@ -2317,7 +878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="2">
         <v>43397</v>
       </c>
@@ -2331,7 +892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="5">
         <v>43397</v>
       </c>
@@ -2345,7 +906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="2">
         <v>43397</v>
       </c>
@@ -2359,7 +920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="5">
         <v>43397</v>
       </c>
@@ -2373,7 +934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="2">
         <v>43399</v>
       </c>
@@ -2387,7 +948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="5">
         <v>43399</v>
       </c>
@@ -2401,7 +962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="2">
         <v>43399</v>
       </c>
@@ -2415,7 +976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="5">
         <v>43399</v>
       </c>
@@ -2429,7 +990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" s="2">
         <v>43399</v>
       </c>
@@ -2443,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" s="5">
         <v>43399</v>
       </c>
@@ -2457,7 +1018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="2">
         <v>43402</v>
       </c>
@@ -2471,7 +1032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" s="5">
         <v>43402</v>
       </c>
@@ -2485,7 +1046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" s="2">
         <v>43402</v>
       </c>
@@ -2499,7 +1060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="5">
         <v>43402</v>
       </c>
@@ -2513,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="2">
         <v>43402</v>
       </c>
@@ -2527,7 +1088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" s="5">
         <v>43402</v>
       </c>
@@ -2541,7 +1102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="2">
         <v>43402</v>
       </c>
@@ -2555,7 +1116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="5">
         <v>43402</v>
       </c>
@@ -2569,7 +1130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="2">
         <v>43402</v>
       </c>
@@ -2583,7 +1144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="5">
         <v>43402</v>
       </c>
@@ -2597,7 +1158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="2">
         <v>43402</v>
       </c>
@@ -2611,7 +1172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="5">
         <v>43402</v>
       </c>
@@ -2625,7 +1186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="2">
         <v>43402</v>
       </c>
@@ -2639,7 +1200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="5">
         <v>43402</v>
       </c>
@@ -2653,7 +1214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="2">
         <v>43402</v>
       </c>
@@ -2667,7 +1228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="5">
         <v>43402</v>
       </c>
@@ -2681,7 +1242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="2">
         <v>43402</v>
       </c>
@@ -2695,7 +1256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="5">
         <v>43402</v>
       </c>
@@ -2709,7 +1270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="2">
         <v>43402</v>
       </c>
@@ -2723,7 +1284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="5">
         <v>43405</v>
       </c>
@@ -2737,7 +1298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="2">
         <v>43405</v>
       </c>
@@ -2751,7 +1312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="5">
         <v>43405</v>
       </c>
@@ -2765,7 +1326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="2">
         <v>43409</v>
       </c>
@@ -2779,7 +1340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="5">
         <v>43409</v>
       </c>
@@ -2793,7 +1354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="2">
         <v>43409</v>
       </c>
@@ -2807,7 +1368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="5">
         <v>43409</v>
       </c>
@@ -2821,7 +1382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="2">
         <v>43409</v>
       </c>
@@ -2835,7 +1396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" s="5">
         <v>43410</v>
       </c>
@@ -2849,7 +1410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" s="2">
         <v>43410</v>
       </c>
@@ -2863,7 +1424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" s="5">
         <v>43410</v>
       </c>
@@ -2877,7 +1438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" s="2">
         <v>43410</v>
       </c>
@@ -2891,7 +1452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61" s="5">
         <v>43410</v>
       </c>
@@ -2905,7 +1466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62" s="2">
         <v>43410</v>
       </c>
@@ -2919,7 +1480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63" s="5">
         <v>43410</v>
       </c>
@@ -2933,7 +1494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64" s="2">
         <v>43410</v>
       </c>
@@ -2947,7 +1508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="A65" s="5">
         <v>43410</v>
       </c>
@@ -2961,7 +1522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="A66" s="2">
         <v>43411</v>
       </c>
@@ -2975,7 +1536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67" s="5">
         <v>43411</v>
       </c>
@@ -2989,7 +1550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4">
       <c r="A68" s="2">
         <v>43411</v>
       </c>
@@ -3003,7 +1564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="A69" s="5">
         <v>43411</v>
       </c>
@@ -3017,7 +1578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4">
       <c r="A70" s="2">
         <v>43411</v>
       </c>
@@ -3031,7 +1592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71" s="5">
         <v>43411</v>
       </c>
@@ -3045,7 +1606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72" s="2">
         <v>43411</v>
       </c>
@@ -3059,7 +1620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4">
       <c r="A73" s="5">
         <v>43412</v>
       </c>
@@ -3073,7 +1634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4">
       <c r="A74" s="2">
         <v>43412</v>
       </c>
@@ -3087,7 +1648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4">
       <c r="A75" s="5">
         <v>43412</v>
       </c>
@@ -3101,7 +1662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4">
       <c r="A76" s="2">
         <v>43412</v>
       </c>
@@ -3115,7 +1676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4">
       <c r="A77" s="5">
         <v>43412</v>
       </c>
@@ -3129,7 +1690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4">
       <c r="A78" s="2">
         <v>43412</v>
       </c>
@@ -3143,7 +1704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4">
       <c r="A79" s="5">
         <v>43413</v>
       </c>
@@ -3157,7 +1718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4">
       <c r="A80" s="2">
         <v>43413</v>
       </c>
@@ -3171,7 +1732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4">
       <c r="A81" s="5">
         <v>43413</v>
       </c>
@@ -3185,7 +1746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4">
       <c r="A82" s="2">
         <v>43413</v>
       </c>
@@ -3199,7 +1760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4">
       <c r="A83" s="5">
         <v>43417</v>
       </c>
@@ -3213,7 +1774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4">
       <c r="A84" s="2">
         <v>43417</v>
       </c>
@@ -3227,7 +1788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4">
       <c r="A85" s="5">
         <v>43417</v>
       </c>
@@ -3241,7 +1802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4">
       <c r="A86" s="2">
         <v>43417</v>
       </c>
@@ -3255,7 +1816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4">
       <c r="A87" s="5">
         <v>43418</v>
       </c>
@@ -3269,7 +1830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4">
       <c r="A88" s="2">
         <v>43418</v>
       </c>
@@ -3283,7 +1844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4">
       <c r="A89" s="5">
         <v>43418</v>
       </c>
@@ -3297,7 +1858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4">
       <c r="A90" s="2">
         <v>43418</v>
       </c>
@@ -3311,7 +1872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4">
       <c r="A91" s="5">
         <v>43419</v>
       </c>
@@ -3325,7 +1886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4">
       <c r="A92" s="2">
         <v>43419</v>
       </c>
@@ -3339,7 +1900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4">
       <c r="A93" s="5">
         <v>43419</v>
       </c>
@@ -3353,7 +1914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4">
       <c r="A94" s="2">
         <v>43419</v>
       </c>
@@ -3367,7 +1928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4">
       <c r="A95" s="5">
         <v>43419</v>
       </c>
@@ -3381,7 +1942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4">
       <c r="A96" s="2">
         <v>43419</v>
       </c>
@@ -3395,7 +1956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4">
       <c r="A97" s="5">
         <v>43420</v>
       </c>
@@ -3409,7 +1970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4">
       <c r="A98" s="2">
         <v>43420</v>
       </c>
@@ -3423,7 +1984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4">
       <c r="A99" s="5">
         <v>43420</v>
       </c>
@@ -3437,7 +1998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4">
       <c r="A100" s="2">
         <v>43420</v>
       </c>
@@ -3451,7 +2012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4">
       <c r="A101" s="5">
         <v>43420</v>
       </c>
@@ -3465,7 +2026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4">
       <c r="A102" s="2">
         <v>43421</v>
       </c>
@@ -3479,7 +2040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4">
       <c r="A103" s="5">
         <v>43421</v>
       </c>
@@ -3493,7 +2054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4">
       <c r="A104" s="2">
         <v>43421</v>
       </c>
@@ -3507,7 +2068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4">
       <c r="A105" s="5">
         <v>43421</v>
       </c>
@@ -3521,7 +2082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4">
       <c r="A106" s="2">
         <v>43421</v>
       </c>
@@ -3535,7 +2096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4">
       <c r="A107" s="5">
         <v>43424</v>
       </c>
@@ -3549,7 +2110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4">
       <c r="A108" s="2">
         <v>43424</v>
       </c>
@@ -3563,7 +2124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4">
       <c r="A109" s="5">
         <v>43424</v>
       </c>
@@ -3577,7 +2138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4">
       <c r="A110" s="2">
         <v>43424</v>
       </c>
@@ -3591,7 +2152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4">
       <c r="A111" s="5">
         <v>43424</v>
       </c>
@@ -3605,7 +2166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4">
       <c r="A112" s="2">
         <v>43424</v>
       </c>
@@ -3619,7 +2180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4">
       <c r="A113" s="5">
         <v>43424</v>
       </c>
@@ -3633,7 +2194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4">
       <c r="A114" s="2">
         <v>43424</v>
       </c>
@@ -3647,7 +2208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4">
       <c r="A115" s="5">
         <v>43425</v>
       </c>
@@ -3661,7 +2222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4">
       <c r="A116" s="2">
         <v>43426</v>
       </c>
@@ -3675,7 +2236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4">
       <c r="A117" s="5">
         <v>43426</v>
       </c>
@@ -3689,7 +2250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4">
       <c r="A118" s="2">
         <v>43426</v>
       </c>
@@ -3703,1337 +2264,1505 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="C120" s="8" t="s">
+    <row r="119" spans="1:4">
+      <c r="A119" s="5">
+        <v>43427</v>
+      </c>
+      <c r="B119" s="6">
+        <v>15</v>
+      </c>
+      <c r="C119" s="6">
+        <v>17</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="2">
+        <v>43427</v>
+      </c>
+      <c r="B120" s="3">
+        <v>16</v>
+      </c>
+      <c r="C120" s="3">
+        <v>18</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="5">
+        <v>43427</v>
+      </c>
+      <c r="B121" s="6">
+        <v>9</v>
+      </c>
+      <c r="C121" s="6">
+        <v>15</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="2">
+        <v>43427</v>
+      </c>
+      <c r="B122" s="3">
+        <v>9</v>
+      </c>
+      <c r="C122" s="3">
+        <v>15</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="5">
+        <v>43427</v>
+      </c>
+      <c r="B123" s="6">
+        <v>12</v>
+      </c>
+      <c r="C123" s="6">
+        <v>15</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="2">
+        <v>43427</v>
+      </c>
+      <c r="B124" s="3">
+        <v>7</v>
+      </c>
+      <c r="C124" s="3">
+        <v>15</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="5">
+        <v>43427</v>
+      </c>
+      <c r="B125" s="6">
+        <v>12</v>
+      </c>
+      <c r="C125" s="6">
+        <v>15</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="C127" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D120" s="8" t="s">
+      <c r="D127" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A121" s="18" t="s">
+    <row r="128" spans="1:4">
+      <c r="A128" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B121" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C121" s="10">
+      <c r="B128" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C128" s="11">
         <v>27</v>
       </c>
-      <c r="D121" s="11">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A122" s="18" t="s">
+      <c r="D128" s="12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B122" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C122" s="10">
+      <c r="B129" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C129" s="11">
         <v>33</v>
       </c>
-      <c r="D122" s="11">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="18" t="s">
+      <c r="D129" s="12">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B123" s="12" t="s">
+      <c r="B130" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C123" s="13">
+      <c r="C130" s="14">
         <v>60</v>
       </c>
-      <c r="D123" s="14">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A124" s="18" t="s">
+      <c r="D130" s="15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B124" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C124" s="15">
+      <c r="B131" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131" s="16">
+        <v>42.19</v>
+      </c>
+      <c r="D131" s="17">
         <v>45</v>
       </c>
-      <c r="D124" s="16">
-        <v>43.1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A125" s="18" t="s">
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B125" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C125" s="15">
-        <v>56.9</v>
-      </c>
-      <c r="D125" s="16">
+      <c r="B132" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C132" s="16">
         <v>55</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A126" s="18" t="s">
+      <c r="D132" s="17">
+        <v>57.81</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B126" s="12" t="s">
+      <c r="B133" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C126" s="17">
-        <v>50.85</v>
-      </c>
-      <c r="D126" s="12">
-        <v>49.15</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A127" s="18" t="s">
+      <c r="C133" s="18">
+        <v>48.39</v>
+      </c>
+      <c r="D133" s="13">
+        <v>51.61</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B127" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C127" s="15">
-        <v>12.87</v>
-      </c>
-      <c r="D127" s="16">
-        <v>13.33</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A128" s="18" t="s">
+      <c r="B134" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C134" s="16">
+        <v>12.81</v>
+      </c>
+      <c r="D134" s="17">
+        <v>13.65</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B128" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C128" s="15">
-        <v>13.52</v>
-      </c>
-      <c r="D128" s="16">
-        <v>13.55</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A129" s="18" t="s">
+      <c r="B135" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C135" s="16">
+        <v>13.58</v>
+      </c>
+      <c r="D135" s="17">
+        <v>13.67</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B129" s="12" t="s">
+      <c r="B136" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C129" s="17">
+      <c r="C136" s="18">
         <v>13.19</v>
       </c>
-      <c r="D129" s="12">
-        <v>13.44</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A130" s="18" t="s">
+      <c r="D136" s="13">
+        <v>13.66</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B130" s="9" t="s">
+      <c r="B137" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C130" s="10">
+      <c r="C137" s="11">
         <v>0</v>
       </c>
-      <c r="D130" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A131" s="18" t="s">
+      <c r="D137" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B131" s="9" t="s">
+      <c r="B138" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C131" s="10">
+      <c r="C138" s="11">
         <v>7</v>
       </c>
-      <c r="D131" s="11">
-        <v>6</v>
+      <c r="D138" s="12">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A121:A123"/>
-    <mergeCell ref="A124:A126"/>
-    <mergeCell ref="A127:A129"/>
-    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="A128:A130"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="A134:A136"/>
+    <mergeCell ref="A137:A138"/>
   </mergeCells>
   <conditionalFormatting sqref="B10">
-    <cfRule type="cellIs" dxfId="233" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100">
-    <cfRule type="cellIs" dxfId="232" priority="197" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="197" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101">
-    <cfRule type="cellIs" dxfId="231" priority="199" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="199" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B102">
-    <cfRule type="cellIs" dxfId="230" priority="201" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="201" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B103">
-    <cfRule type="cellIs" dxfId="229" priority="203" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="203" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B104">
-    <cfRule type="cellIs" dxfId="228" priority="205" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="205" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B105">
-    <cfRule type="cellIs" dxfId="227" priority="207" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="207" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B106">
-    <cfRule type="cellIs" dxfId="226" priority="209" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="209" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B107">
-    <cfRule type="cellIs" dxfId="225" priority="211" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="211" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B108">
-    <cfRule type="cellIs" dxfId="224" priority="213" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="213" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B109">
-    <cfRule type="cellIs" dxfId="223" priority="215" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="215" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="cellIs" dxfId="222" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="19" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B110">
-    <cfRule type="cellIs" dxfId="221" priority="217" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="217" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B111">
-    <cfRule type="cellIs" dxfId="220" priority="219" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="219" operator="greaterThan">
       <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B112">
-    <cfRule type="cellIs" dxfId="219" priority="221" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="221" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113">
-    <cfRule type="cellIs" dxfId="218" priority="223" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="223" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114">
-    <cfRule type="cellIs" dxfId="217" priority="225" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="225" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115">
-    <cfRule type="cellIs" dxfId="216" priority="227" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="227" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B116">
-    <cfRule type="cellIs" dxfId="215" priority="229" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="229" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B117">
-    <cfRule type="cellIs" dxfId="214" priority="231" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="231" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B118">
-    <cfRule type="cellIs" dxfId="213" priority="233" operator="greaterThan">
-      <formula>15</formula>
+    <cfRule type="cellIs" dxfId="0" priority="233" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B119">
+    <cfRule type="cellIs" dxfId="0" priority="235" operator="greaterThan">
+      <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="212" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B120">
+    <cfRule type="cellIs" dxfId="0" priority="237" operator="greaterThan">
+      <formula>18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B121">
+    <cfRule type="cellIs" dxfId="0" priority="239" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B122">
+    <cfRule type="cellIs" dxfId="0" priority="241" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B123">
+    <cfRule type="cellIs" dxfId="0" priority="243" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B124">
+    <cfRule type="cellIs" dxfId="0" priority="245" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
+    <cfRule type="cellIs" dxfId="0" priority="247" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="211" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="23" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="210" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="25" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="cellIs" dxfId="209" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="27" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="cellIs" dxfId="208" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="29" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="cellIs" dxfId="207" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="31" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="cellIs" dxfId="206" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="33" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="205" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="35" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="204" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="203" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="37" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="202" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="39" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="cellIs" dxfId="201" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="41" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="cellIs" dxfId="200" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="43" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="199" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="45" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="cellIs" dxfId="198" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="47" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="cellIs" dxfId="197" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="49" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="196" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="51" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="195" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="53" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="194" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="55" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="193" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="192" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="57" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="cellIs" dxfId="191" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="59" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="190" priority="61" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="61" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="cellIs" dxfId="189" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="63" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="cellIs" dxfId="188" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="65" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="cellIs" dxfId="187" priority="67" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="67" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="186" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="69" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="cellIs" dxfId="185" priority="71" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="71" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="cellIs" dxfId="184" priority="73" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="73" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="cellIs" dxfId="183" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="75" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="182" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="cellIs" dxfId="181" priority="77" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="77" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="cellIs" dxfId="180" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="79" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="cellIs" dxfId="179" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="81" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="178" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="83" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="177" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="85" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="176" priority="87" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="87" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="175" priority="89" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="89" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="cellIs" dxfId="174" priority="91" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="91" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="cellIs" dxfId="173" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="93" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="cellIs" dxfId="172" priority="95" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="95" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="171" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="cellIs" dxfId="170" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="97" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" dxfId="169" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="99" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="cellIs" dxfId="168" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="101" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="cellIs" dxfId="167" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="103" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="cellIs" dxfId="166" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="105" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="cellIs" dxfId="165" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="107" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="cellIs" dxfId="164" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="109" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="163" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="111" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="cellIs" dxfId="162" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="113" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="cellIs" dxfId="161" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="115" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="160" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="cellIs" dxfId="159" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="117" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="cellIs" dxfId="158" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="119" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="cellIs" dxfId="157" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="121" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="cellIs" dxfId="156" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="123" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="cellIs" dxfId="155" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="125" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="cellIs" dxfId="154" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="127" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="cellIs" dxfId="153" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="129" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67">
-    <cfRule type="cellIs" dxfId="152" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="131" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68">
-    <cfRule type="cellIs" dxfId="151" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="133" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69">
-    <cfRule type="cellIs" dxfId="150" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="135" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="149" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="cellIs" dxfId="148" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="137" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71">
-    <cfRule type="cellIs" dxfId="147" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="139" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72">
-    <cfRule type="cellIs" dxfId="146" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="141" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73">
-    <cfRule type="cellIs" dxfId="145" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="143" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74">
-    <cfRule type="cellIs" dxfId="144" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="145" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="cellIs" dxfId="143" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="147" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="cellIs" dxfId="142" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="149" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="cellIs" dxfId="141" priority="151" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="151" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="cellIs" dxfId="140" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="153" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="cellIs" dxfId="139" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="155" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="138" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80">
-    <cfRule type="cellIs" dxfId="137" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="157" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81">
-    <cfRule type="cellIs" dxfId="136" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="159" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82">
-    <cfRule type="cellIs" dxfId="135" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="161" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="cellIs" dxfId="134" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="163" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="cellIs" dxfId="133" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="165" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85">
-    <cfRule type="cellIs" dxfId="132" priority="167" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="167" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="cellIs" dxfId="131" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="169" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="cellIs" dxfId="130" priority="171" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="171" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="cellIs" dxfId="129" priority="173" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="173" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="cellIs" dxfId="128" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="175" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="127" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="cellIs" dxfId="126" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="177" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="cellIs" dxfId="125" priority="179" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="179" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="cellIs" dxfId="124" priority="181" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="181" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="cellIs" dxfId="123" priority="183" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="183" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="cellIs" dxfId="122" priority="185" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="185" operator="greaterThan">
       <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="cellIs" dxfId="121" priority="187" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="187" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96">
-    <cfRule type="cellIs" dxfId="120" priority="189" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="189" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97">
-    <cfRule type="cellIs" dxfId="119" priority="191" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="191" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="cellIs" dxfId="118" priority="193" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="193" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99">
-    <cfRule type="cellIs" dxfId="117" priority="195" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="195" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="116" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100">
-    <cfRule type="cellIs" dxfId="115" priority="198" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="198" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="cellIs" dxfId="114" priority="200" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="200" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102">
-    <cfRule type="cellIs" dxfId="113" priority="202" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="202" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="cellIs" dxfId="112" priority="204" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="204" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="cellIs" dxfId="111" priority="206" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="206" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="cellIs" dxfId="110" priority="208" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="208" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="cellIs" dxfId="109" priority="210" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="210" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107">
-    <cfRule type="cellIs" dxfId="108" priority="212" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="212" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C108">
-    <cfRule type="cellIs" dxfId="107" priority="214" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="214" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C109">
-    <cfRule type="cellIs" dxfId="106" priority="216" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="216" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="105" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="20" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C110">
-    <cfRule type="cellIs" dxfId="104" priority="218" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="218" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C111">
-    <cfRule type="cellIs" dxfId="103" priority="220" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="220" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C112">
-    <cfRule type="cellIs" dxfId="102" priority="222" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="222" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113">
-    <cfRule type="cellIs" dxfId="101" priority="224" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="224" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C114">
-    <cfRule type="cellIs" dxfId="100" priority="226" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="226" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C115">
-    <cfRule type="cellIs" dxfId="99" priority="228" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="228" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C116">
-    <cfRule type="cellIs" dxfId="98" priority="230" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="230" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C117">
-    <cfRule type="cellIs" dxfId="97" priority="232" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="232" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118">
-    <cfRule type="cellIs" dxfId="96" priority="234" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="234" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C119">
+    <cfRule type="cellIs" dxfId="0" priority="236" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="95" priority="22" operator="greaterThan">
-      <formula>15</formula>
+    <cfRule type="cellIs" dxfId="0" priority="22" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C120">
+    <cfRule type="cellIs" dxfId="0" priority="238" operator="greaterThan">
+      <formula>16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C121">
+    <cfRule type="cellIs" dxfId="0" priority="240" operator="greaterThan">
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C122">
+    <cfRule type="cellIs" dxfId="0" priority="242" operator="greaterThan">
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C123">
+    <cfRule type="cellIs" dxfId="0" priority="244" operator="greaterThan">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C124">
+    <cfRule type="cellIs" dxfId="0" priority="246" operator="greaterThan">
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C125">
+    <cfRule type="cellIs" dxfId="0" priority="248" operator="greaterThan">
+      <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="94" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="24" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="93" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="26" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="92" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="28" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="91" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="30" operator="greaterThan">
       <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="90" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="32" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="89" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="34" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="88" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="36" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="87" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="cellIs" dxfId="86" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="38" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="85" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="40" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="84" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="42" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="83" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="44" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="82" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="46" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="cellIs" dxfId="81" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="48" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="80" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="50" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="79" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="52" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="78" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="54" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="77" priority="56" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="56" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="76" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="cellIs" dxfId="75" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="58" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="74" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="60" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="73" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="62" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="72" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="64" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="71" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="66" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="70" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="68" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="69" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="70" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="68" priority="72" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="72" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="cellIs" dxfId="67" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="74" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="cellIs" dxfId="66" priority="76" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="76" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="65" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="64" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="78" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="63" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="80" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="62" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="82" operator="greaterThan">
       <formula>22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="61" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="84" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="60" priority="86" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="86" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="cellIs" dxfId="59" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="88" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="58" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="90" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="57" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="92" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="56" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="94" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="55" priority="96" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="96" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="54" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="53" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="98" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="52" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="100" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="51" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="102" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="cellIs" dxfId="50" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="104" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="49" priority="106" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="106" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
-    <cfRule type="cellIs" dxfId="48" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="108" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="47" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="110" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="cellIs" dxfId="46" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="112" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="cellIs" dxfId="45" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="114" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="44" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="116" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="42" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="118" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="41" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="120" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="40" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="122" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="39" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="124" operator="greaterThan">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="38" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="126" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="cellIs" dxfId="37" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="128" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="cellIs" dxfId="36" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="130" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="cellIs" dxfId="35" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="132" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="cellIs" dxfId="34" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="134" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="cellIs" dxfId="33" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="136" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="32" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="cellIs" dxfId="31" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="138" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="cellIs" dxfId="30" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="140" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72">
-    <cfRule type="cellIs" dxfId="29" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="142" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C73">
-    <cfRule type="cellIs" dxfId="28" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="144" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="27" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="146" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="cellIs" dxfId="26" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="148" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="cellIs" dxfId="25" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="150" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="cellIs" dxfId="24" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="152" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78">
-    <cfRule type="cellIs" dxfId="23" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="154" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79">
-    <cfRule type="cellIs" dxfId="22" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="156" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="21" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80">
-    <cfRule type="cellIs" dxfId="20" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="158" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81">
-    <cfRule type="cellIs" dxfId="19" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="160" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82">
-    <cfRule type="cellIs" dxfId="18" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="162" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="cellIs" dxfId="17" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="164" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84">
-    <cfRule type="cellIs" dxfId="16" priority="166" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="166" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="cellIs" dxfId="15" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="168" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="cellIs" dxfId="14" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="170" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="cellIs" dxfId="13" priority="172" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="172" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88">
-    <cfRule type="cellIs" dxfId="12" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="174" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="cellIs" dxfId="11" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="176" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="9" priority="178" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="178" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="cellIs" dxfId="8" priority="180" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="180" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92">
-    <cfRule type="cellIs" dxfId="7" priority="182" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="182" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
-    <cfRule type="cellIs" dxfId="6" priority="184" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="184" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94">
-    <cfRule type="cellIs" dxfId="5" priority="186" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="186" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="cellIs" dxfId="4" priority="188" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="188" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96">
-    <cfRule type="cellIs" dxfId="3" priority="190" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="190" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="cellIs" dxfId="2" priority="192" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="192" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="1" priority="194" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="194" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated scores, added crap to scratch pad
</commit_message>
<xml_diff>
--- a/assets/excel/ping_pong_scoresheet_v2.xlsx
+++ b/assets/excel/ping_pong_scoresheet_v2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="16">
   <si>
     <t>Fritz</t>
   </si>
@@ -620,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E226"/>
+  <dimension ref="A1:E228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4250,174 +4250,208 @@
         <v>43452.56280092592</v>
       </c>
     </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="2">
+        <v>43453</v>
+      </c>
+      <c r="B214" s="3">
+        <v>15</v>
+      </c>
+      <c r="C214" s="3">
+        <v>13</v>
+      </c>
+      <c r="D214" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E214" s="5">
+        <v>43453.421875</v>
+      </c>
+    </row>
     <row r="215" spans="1:5">
-      <c r="C215" s="10" t="s">
+      <c r="A215" s="6">
+        <v>43453</v>
+      </c>
+      <c r="B215" s="7">
+        <v>15</v>
+      </c>
+      <c r="C215" s="7">
+        <v>10</v>
+      </c>
+      <c r="D215" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E215" s="9">
+        <v>43453.42680555556</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="C217" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D215" s="10" t="s">
+      <c r="D217" s="10" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5">
-      <c r="A216" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B216" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C216" s="13">
-        <v>43</v>
-      </c>
-      <c r="D216" s="14">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5">
-      <c r="A217" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B217" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C217" s="13">
-        <v>48</v>
-      </c>
-      <c r="D217" s="14">
-        <v>69</v>
       </c>
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B218" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C218" s="16">
-        <v>91</v>
-      </c>
-      <c r="D218" s="17">
-        <v>121</v>
+      <c r="B218" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C218" s="13">
+        <v>44</v>
+      </c>
+      <c r="D218" s="14">
+        <v>52</v>
       </c>
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B219" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C219" s="18">
-        <v>38.39</v>
-      </c>
-      <c r="D219" s="19">
-        <v>52</v>
+        <v>5</v>
+      </c>
+      <c r="C219" s="13">
+        <v>49</v>
+      </c>
+      <c r="D219" s="14">
+        <v>69</v>
       </c>
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B220" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C220" s="18">
-        <v>48</v>
-      </c>
-      <c r="D220" s="19">
-        <v>61.61</v>
+        <v>9</v>
+      </c>
+      <c r="B220" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C220" s="16">
+        <v>93</v>
+      </c>
+      <c r="D220" s="17">
+        <v>121</v>
       </c>
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B221" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C221" s="20">
-        <v>42.92</v>
-      </c>
-      <c r="D221" s="15">
-        <v>57.08</v>
+      <c r="B221" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C221" s="18">
+        <v>38.94</v>
+      </c>
+      <c r="D221" s="19">
+        <v>51.49</v>
       </c>
     </row>
     <row r="222" spans="1:5">
       <c r="A222" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B222" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C222" s="18">
-        <v>12.63</v>
+        <v>48.51</v>
       </c>
       <c r="D222" s="19">
-        <v>13.53</v>
+        <v>61.06</v>
       </c>
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B223" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C223" s="18">
-        <v>13.2</v>
-      </c>
-      <c r="D223" s="19">
-        <v>13.97</v>
+        <v>10</v>
+      </c>
+      <c r="B223" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C223" s="20">
+        <v>43.46</v>
+      </c>
+      <c r="D223" s="15">
+        <v>56.54</v>
       </c>
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B224" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C224" s="20">
-        <v>12.9</v>
-      </c>
-      <c r="D224" s="15">
-        <v>13.76</v>
+      <c r="B224" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C224" s="18">
+        <v>12.65</v>
+      </c>
+      <c r="D224" s="19">
+        <v>13.5</v>
       </c>
     </row>
     <row r="225" spans="1:4">
       <c r="A225" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B225" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C225" s="13">
-        <v>0</v>
-      </c>
-      <c r="D225" s="14">
-        <v>5</v>
+        <v>5</v>
+      </c>
+      <c r="C225" s="18">
+        <v>13.22</v>
+      </c>
+      <c r="D225" s="19">
+        <v>13.96</v>
       </c>
     </row>
     <row r="226" spans="1:4">
       <c r="A226" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B226" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C226" s="20">
+        <v>12.92</v>
+      </c>
+      <c r="D226" s="15">
+        <v>13.74</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B226" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C226" s="13">
+      <c r="B227" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C227" s="13">
+        <v>2</v>
+      </c>
+      <c r="D227" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B228" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C228" s="13">
         <v>7</v>
       </c>
-      <c r="D226" s="14">
+      <c r="D228" s="14">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A216:A218"/>
-    <mergeCell ref="A219:A221"/>
-    <mergeCell ref="A222:A224"/>
-    <mergeCell ref="A225:A226"/>
+    <mergeCell ref="A218:A220"/>
+    <mergeCell ref="A221:A223"/>
+    <mergeCell ref="A224:A226"/>
+    <mergeCell ref="A227:A228"/>
   </mergeCells>
   <conditionalFormatting sqref="B10">
     <cfRule type="cellIs" dxfId="0" priority="17" operator="greaterThan">
@@ -5054,6 +5088,16 @@
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B214">
+    <cfRule type="cellIs" dxfId="0" priority="425" operator="greaterThan">
+      <formula>13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B215">
+    <cfRule type="cellIs" dxfId="0" priority="427" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B22">
     <cfRule type="cellIs" dxfId="0" priority="41" operator="greaterThan">
       <formula>15</formula>
@@ -6114,6 +6158,16 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C214">
+    <cfRule type="cellIs" dxfId="0" priority="426" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C215">
+    <cfRule type="cellIs" dxfId="0" priority="428" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C22">
     <cfRule type="cellIs" dxfId="0" priority="42" operator="greaterThan">
       <formula>7</formula>

</xml_diff>